<commit_message>
Update parameters to HYEFU23, and using the fixed template (fixing Accommodation Supplement parameters)
</commit_message>
<xml_diff>
--- a/inst/MFTC_calculator/App_Parameters/IncomeExplorer_TY14.xlsx
+++ b/inst/MFTC_calculator/App_Parameters/IncomeExplorer_TY14.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>Parameter</t>
   </si>
@@ -39,30 +39,6 @@
     <t>Accommodation/BaseRateThreshold/Rent</t>
   </si>
   <si>
-    <t>Accommodation/MaxRate/CoupleDeps_Single2_Deps/Area1</t>
-  </si>
-  <si>
-    <t>Accommodation/MaxRate/CoupleDeps_Single2_Deps/Area2</t>
-  </si>
-  <si>
-    <t>Accommodation/MaxRate/CoupleDeps_Single2_Deps/Area3</t>
-  </si>
-  <si>
-    <t>Accommodation/MaxRate/CoupleDeps_Single2_Deps/Area4</t>
-  </si>
-  <si>
-    <t>Accommodation/MaxRate/CoupleNoDeps_Single1Dep/Area1</t>
-  </si>
-  <si>
-    <t>Accommodation/MaxRate/CoupleNoDeps_Single1Dep/Area2</t>
-  </si>
-  <si>
-    <t>Accommodation/MaxRate/CoupleNoDeps_Single1Dep/Area3</t>
-  </si>
-  <si>
-    <t>Accommodation/MaxRate/CoupleNoDeps_Single1Dep/Area4</t>
-  </si>
-  <si>
     <t>Accommodation/MaxRate/SingleNoDeps/Area1</t>
   </si>
   <si>
@@ -111,15 +87,9 @@
     <t>Benefits/WinterEnergy/Rates/CoupleOrDeps</t>
   </si>
   <si>
-    <t>Benefits/LivingAlonePayment/Single</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
-    <t>Benefits/LivingAlonePayment/SoleParent</t>
-  </si>
-  <si>
     <t>FamilyAssistance/Abatement/AbatementScale</t>
   </si>
   <si>
@@ -159,21 +129,9 @@
     <t>IETC/OnlyFamiliesWithoutChildren</t>
   </si>
   <si>
-    <t>EITC/ApplyEITC</t>
-  </si>
-  <si>
-    <t>EITC/AbatementScale</t>
-  </si>
-  <si>
-    <t>EITC/ExcludeFamiliesWithoutChildren</t>
-  </si>
-  <si>
     <t>Tax/BaseScale</t>
   </si>
   <si>
-    <t>[['0';'0'];['0';'0']]</t>
-  </si>
-  <si>
     <t>FamilyAssistance/IWTC/IncomeThreshold/Single</t>
   </si>
   <si>
@@ -216,9 +174,6 @@
     <t>Sole Parent Support settings</t>
   </si>
   <si>
-    <t xml:space="preserve">Living alone payment, given to single people receiving a core benefit and not sharing accommodation with another adult </t>
-  </si>
-  <si>
     <t>FamilyAssistance/FTC/Rates/FirstChild</t>
   </si>
   <si>
@@ -255,9 +210,6 @@
     <t>Rate is specified with each forecast update</t>
   </si>
   <si>
-    <t xml:space="preserve">Living alone payment, given to sole parents receiving a core benefit and not sharing accommodation with another adult </t>
-  </si>
-  <si>
     <t>Specified with each forecast update</t>
   </si>
   <si>
@@ -279,15 +231,6 @@
     <t>Number of hours for a single parent to be classified as working full time, for IWTC and MFTC eligibility (FamilyAssistance/IWTC/Eligibility must be set to 0)</t>
   </si>
   <si>
-    <t>Single parent phase-in scale for IWTC, eg a phase-in scale of 20% is specifed as -0.2 (FamilyAssistance/IWTC/Eligibility must be set to 2)</t>
-  </si>
-  <si>
-    <t>Couple phase-in scale for IWTC, eg a phase-in scale of 20% is specifed as -0.2 (FamilyAssistance/IWTC/Eligibility must be set to 2)</t>
-  </si>
-  <si>
-    <t>Eligibilty test for In Work Tax Credit. 0: Status quo, based on hours worked and not given to beneficiaries. 1: Income test, option to give to beneficiaries (see below), 2: Phase in amount of IWTC based on phase-in scales (see below).</t>
-  </si>
-  <si>
     <t>Minimum income that ensures that a family is better off in work than on benefit; the Minimum Family Tax Credit brings their income up to this amount. Value is calculated by the TAWA version of the IRD calculator.</t>
   </si>
   <si>
@@ -297,21 +240,9 @@
     <t>Independent Earner Tax Credit, abatement scale</t>
   </si>
   <si>
-    <t>Independent Earner Tax Credit, minimum bound on earned income to determine eligability</t>
-  </si>
-  <si>
     <t>Independent Earner Tax Credit, amount for each year</t>
   </si>
   <si>
-    <t>Earned Income Tax Credit, switch to turn on</t>
-  </si>
-  <si>
-    <t>Earned Income Tax Credit, abatement scale (includes a phase-in)</t>
-  </si>
-  <si>
-    <t>Earner Income Tax Credit. Switch to exclude families without children</t>
-  </si>
-  <si>
     <t>FamilyAssistance/Abatement/Order</t>
   </si>
   <si>
@@ -321,6 +252,42 @@
     <t>Working for Families abatement</t>
   </si>
   <si>
+    <t>Accommodation/MaxRate/CoupleDeps/Single2/Deps/Area1</t>
+  </si>
+  <si>
+    <t>Accommodation/MaxRate/CoupleDeps/Single2/Deps/Area2</t>
+  </si>
+  <si>
+    <t>Accommodation/MaxRate/CoupleDeps/Single2/Deps/Area3</t>
+  </si>
+  <si>
+    <t>Accommodation/MaxRate/CoupleDeps/Single2/Deps/Area4</t>
+  </si>
+  <si>
+    <t>Accommodation/MaxRate/CoupleNoDeps/Single1Dep/Area1</t>
+  </si>
+  <si>
+    <t>Accommodation/MaxRate/CoupleNoDeps/Single1Dep/Area2</t>
+  </si>
+  <si>
+    <t>Accommodation/MaxRate/CoupleNoDeps/Single1Dep/Area3</t>
+  </si>
+  <si>
+    <t>Accommodation/MaxRate/CoupleNoDeps/Single1Dep/Area4</t>
+  </si>
+  <si>
+    <t>Eligibility test for In Work Tax Credit. 0: Status quo, based on hours worked and not given to beneficiaries. 1: Income test, option to give to beneficiaries (see below), 2: Phase in amount of IWTC based on phase-in scales (see below).</t>
+  </si>
+  <si>
+    <t>Single parent phase-in scale for IWTC, e.g. a phase-in scale of 20% is specified as -0.2 (FamilyAssistance/IWTC/Eligibility must be set to 2)</t>
+  </si>
+  <si>
+    <t>Couple phase-in scale for IWTC, e.g. a phase-in scale of 20% is specified as -0.2 (FamilyAssistance/IWTC/Eligibility must be set to 2)</t>
+  </si>
+  <si>
+    <t>Independent Earner Tax Credit, minimum bound on earned income to determine eligibility</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parameter</t>
   </si>
   <si>
@@ -360,84 +327,105 @@
     <t xml:space="preserve">Accommodation/BaseRateThreshold/Rent</t>
   </si>
   <si>
-    <t xml:space="preserve">Accommodation/MaxRate/CoupleDeps_Single2_Deps/Area1</t>
+    <t xml:space="preserve">Accommodation/MaxRate/CoupleDeps/Single2/Deps/Area1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/CoupleDeps/Single2/Deps/Area2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/CoupleDeps/Single2/Deps/Area3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/CoupleDeps/Single2/Deps/Area4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/CoupleNoDeps/Single1Dep/Area1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/CoupleNoDeps/Single1Dep/Area2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/CoupleNoDeps/Single1Dep/Area3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/CoupleNoDeps/Single1Dep/Area4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/SingleNoDeps/Area1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/SingleNoDeps/Area2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/SingleNoDeps/Area3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/MaxRate/SingleNoDeps/Area4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accommodation/PaymentPercentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefits/JSS/AbatementScale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[['0'; '0']; ['4176'; '0.7']]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefits/JSS/CoupleAbatementScale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[['0'; '0']; ['4176'; '0.35']]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefits/JSS/Rate/Couple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">171.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefits/JSS/Rate/CoupleParent</t>
   </si>
   <si>
     <t xml:space="preserve">0</t>
   </si>
   <si>
-    <t xml:space="preserve">Accommodation/MaxRate/CoupleDeps_Single2_Deps/Area2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/MaxRate/CoupleDeps_Single2_Deps/Area3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/MaxRate/CoupleDeps_Single2_Deps/Area4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/MaxRate/CoupleNoDeps_Single1Dep/Area1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/MaxRate/CoupleNoDeps_Single1Dep/Area2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/MaxRate/CoupleNoDeps_Single1Dep/Area3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/MaxRate/CoupleNoDeps_Single1Dep/Area4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/MaxRate/SingleNoDeps/Area1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/MaxRate/SingleNoDeps/Area2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/MaxRate/SingleNoDeps/Area3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/MaxRate/SingleNoDeps/Area4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation/PaymentPercentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benefits/JSS/AbatementScale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[['0'; '0']; ['4176'; '0.7']]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benefits/JSS/CoupleAbatementScale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[['0'; '0']; ['4176'; '0.35']]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benefits/JSS/Rate/Couple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">171.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benefits/JSS/Rate/CoupleParent</t>
-  </si>
-  <si>
     <t xml:space="preserve">Benefits/JSS/Rate/Single</t>
   </si>
   <si>
@@ -471,12 +459,6 @@
     <t xml:space="preserve">Benefits/WinterEnergy/Rates/CoupleOrDeps</t>
   </si>
   <si>
-    <t xml:space="preserve">Benefits/LivingAlonePayment/Single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benefits/LivingAlonePayment/SoleParent</t>
-  </si>
-  <si>
     <t xml:space="preserve">FamilyAssistance/Abatement/AbatementScale</t>
   </si>
   <si>
@@ -583,18 +565,6 @@
   </si>
   <si>
     <t xml:space="preserve">IETC/OnlyFamiliesWithoutChildren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EITC/ApplyEITC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EITC/AbatementScale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[['0';'0'];['0';'0']]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EITC/ExcludeFamiliesWithoutChildren</t>
   </si>
   <si>
     <t xml:space="preserve">Tax/BaseScale</t>
@@ -606,7 +576,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="4">
     <font>
@@ -719,19 +689,20 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1021,669 +992,614 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="true" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="50.6328125" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="50.54296875" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="53.54296875" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="182.08984375" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="182.1796875" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="B2" s="18" t="s">
-        <v>102</v>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" ht="17.149999999999999" customHeight="1">
+      <c r="B2" s="19" t="s">
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="14" t="s">
-        <v>106</v>
+      <c r="B4" s="15" t="s">
+        <v>95</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="15" t="s">
-        <v>108</v>
+      <c r="B5" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="17" t="s">
-        <v>110</v>
+      <c r="B6" s="18" t="s">
+        <v>99</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="10" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="10" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="10" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="10" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="10" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="10" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="10" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="10" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="10" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="10" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="10" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="11" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="17" t="s">
-        <v>145</v>
+      <c r="B28" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C29" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" s="16" t="s">
-        <v>148</v>
-      </c>
       <c r="C30" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" s="15" t="s">
+      <c r="C34" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" s="17" t="s">
+      <c r="C35" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>101</v>
+      <c r="D35" s="9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" s="11" t="s">
+      <c r="D37" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C38" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="B38" s="11" t="s">
+      <c r="D38" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>84</v>
+      <c r="C39" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" s="10" t="s">
+      <c r="D47" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" s="16" t="s">
+      <c r="D48" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>91</v>
+      <c r="C49" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C52" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D52" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D53" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="51">
-      <c r="B51" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="B53" s="14" t="s">
+    <row r="54">
+      <c r="B54" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C54" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="B54" s="11" t="s">
+      <c r="C55" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C54" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="B57" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="B58" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="B59" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="B60" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>78</v>
+      <c r="D55" s="13" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>